<commit_message>
develop: Google Spreadsheet updated
</commit_message>
<xml_diff>
--- a/data/programs.xlsx
+++ b/data/programs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iasonov/Programming/Python/HSE_dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C0736CC-320F-F64B-90FD-2A44CAEC2339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C5D8E31-05F0-A541-AA79-5FA13A8F1556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="16440" xr2:uid="{459C6DFD-26EB-1040-9D7C-59DC53018D97}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16460" xr2:uid="{459C6DFD-26EB-1040-9D7C-59DC53018D97}"/>
   </bookViews>
   <sheets>
     <sheet name="programs" sheetId="1" r:id="rId1"/>
@@ -797,11 +797,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1119,8 +1118,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G8" workbookViewId="0">
-      <selection activeCell="H182" sqref="H182"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="E195" sqref="E195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1151,7 +1150,7 @@
       <c r="F1" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" t="s">
         <v>235</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -1267,7 +1266,7 @@
       <c r="F8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8">
         <v>50</v>
       </c>
       <c r="H8" s="1" t="s">
@@ -1308,7 +1307,7 @@
       <c r="F10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10">
         <v>100</v>
       </c>
       <c r="H10" s="1" t="s">
@@ -1619,7 +1618,7 @@
       <c r="F30" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G30" s="2">
+      <c r="G30">
         <v>100</v>
       </c>
       <c r="H30" s="1" t="s">
@@ -1645,7 +1644,7 @@
       <c r="F31" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G31" s="2">
+      <c r="G31">
         <v>50</v>
       </c>
       <c r="H31" s="1" t="s">
@@ -1719,19 +1718,19 @@
       <c r="B36" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36">
         <v>430</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D36">
         <v>100</v>
       </c>
-      <c r="E36" s="2">
+      <c r="E36">
         <v>1</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G36" s="2">
+      <c r="G36">
         <v>100</v>
       </c>
       <c r="H36" s="1" t="s">
@@ -1802,7 +1801,7 @@
       <c r="F40" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G40" s="2">
+      <c r="G40">
         <v>100</v>
       </c>
       <c r="H40" s="1" t="s">
@@ -1816,19 +1815,19 @@
       <c r="B41" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41">
         <v>490</v>
       </c>
-      <c r="D41" s="2">
+      <c r="D41">
         <v>160</v>
       </c>
-      <c r="E41" s="2">
+      <c r="E41">
         <v>5</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G41" s="2">
+      <c r="G41">
         <v>100</v>
       </c>
       <c r="H41" s="1" t="s">
@@ -1854,7 +1853,7 @@
       <c r="F42" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G42" s="2">
+      <c r="G42">
         <v>100</v>
       </c>
       <c r="H42" s="1" t="s">
@@ -1913,19 +1912,19 @@
       <c r="B46" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46">
         <v>380</v>
       </c>
-      <c r="D46" s="2">
+      <c r="D46">
         <v>70</v>
       </c>
-      <c r="E46" s="2">
+      <c r="E46">
         <v>2</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G46" s="2">
+      <c r="G46">
         <v>100</v>
       </c>
       <c r="H46" s="1" t="s">
@@ -1951,7 +1950,7 @@
       <c r="F47" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G47" s="2">
+      <c r="G47">
         <v>50</v>
       </c>
       <c r="H47" s="1" t="s">
@@ -2040,19 +2039,19 @@
       <c r="B53" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C53" s="2">
-        <v>0</v>
-      </c>
-      <c r="D53" s="2">
-        <v>0</v>
-      </c>
-      <c r="E53" s="2">
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
         <v>0</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G53" s="2">
+      <c r="G53">
         <v>100</v>
       </c>
     </row>
@@ -2195,7 +2194,7 @@
       <c r="F62" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G62" s="2">
+      <c r="G62">
         <v>50</v>
       </c>
     </row>
@@ -2248,7 +2247,7 @@
       <c r="F65" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G65" s="2">
+      <c r="G65">
         <v>100</v>
       </c>
       <c r="H65" s="1" t="s">
@@ -2274,7 +2273,7 @@
       <c r="F66" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G66" s="2">
+      <c r="G66">
         <v>100</v>
       </c>
       <c r="H66" s="1" t="s">
@@ -2315,7 +2314,7 @@
       <c r="F68" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G68" s="2">
+      <c r="G68">
         <v>100</v>
       </c>
       <c r="H68" s="1" t="s">
@@ -2449,19 +2448,19 @@
       <c r="B77" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C77" s="2">
+      <c r="C77">
         <v>510</v>
       </c>
-      <c r="D77" s="2">
+      <c r="D77">
         <v>150</v>
       </c>
-      <c r="E77" s="2">
+      <c r="E77">
         <v>15</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="G77" s="2">
+      <c r="G77">
         <v>100</v>
       </c>
       <c r="H77" s="1" t="s">
@@ -2865,19 +2864,19 @@
       <c r="B104" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C104" s="2">
+      <c r="C104">
         <v>440</v>
       </c>
-      <c r="D104" s="2">
+      <c r="D104">
         <v>5</v>
       </c>
-      <c r="E104" s="2">
+      <c r="E104">
         <v>2</v>
       </c>
       <c r="F104" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G104" s="2">
+      <c r="G104">
         <v>100</v>
       </c>
       <c r="H104" s="1" t="s">
@@ -2951,19 +2950,19 @@
       <c r="B109" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C109" s="2">
+      <c r="C109">
         <v>400</v>
       </c>
-      <c r="D109" s="2">
+      <c r="D109">
         <v>20</v>
       </c>
-      <c r="E109" s="2">
+      <c r="E109">
         <v>1</v>
       </c>
       <c r="F109" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G109" s="2">
+      <c r="G109">
         <v>100</v>
       </c>
       <c r="H109" s="1" t="s">
@@ -2992,19 +2991,19 @@
       <c r="B111" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C111" s="2">
+      <c r="C111">
         <v>700</v>
       </c>
-      <c r="D111" s="2">
+      <c r="D111">
         <v>130</v>
       </c>
-      <c r="E111" s="2">
+      <c r="E111">
         <v>10</v>
       </c>
       <c r="F111" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="G111" s="2">
+      <c r="G111">
         <v>100</v>
       </c>
       <c r="H111" s="1" t="s">
@@ -3018,19 +3017,19 @@
       <c r="B112" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C112" s="2">
+      <c r="C112">
         <v>800</v>
       </c>
-      <c r="D112" s="2">
+      <c r="D112">
         <v>165</v>
       </c>
-      <c r="E112" s="2">
+      <c r="E112">
         <v>10</v>
       </c>
       <c r="F112" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="G112" s="2">
+      <c r="G112">
         <v>100</v>
       </c>
       <c r="H112" s="1" t="s">
@@ -3524,19 +3523,19 @@
       <c r="B145" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C145" s="2">
+      <c r="C145">
         <v>430</v>
       </c>
-      <c r="D145" s="2">
+      <c r="D145">
         <v>100</v>
       </c>
-      <c r="E145" s="2">
+      <c r="E145">
         <v>1</v>
       </c>
       <c r="F145" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G145" s="2">
+      <c r="G145">
         <v>100</v>
       </c>
       <c r="H145" s="1" t="s">
@@ -3580,19 +3579,19 @@
       <c r="B148" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C148" s="2">
+      <c r="C148">
         <v>410</v>
       </c>
-      <c r="D148" s="2">
+      <c r="D148">
         <v>160</v>
       </c>
-      <c r="E148" s="2">
+      <c r="E148">
         <v>10</v>
       </c>
       <c r="F148" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G148" s="2">
+      <c r="G148">
         <v>100</v>
       </c>
       <c r="H148" s="1" t="s">
@@ -3663,7 +3662,7 @@
       <c r="F152" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G152" s="2">
+      <c r="G152">
         <v>100</v>
       </c>
       <c r="H152" s="1" t="s">
@@ -3734,7 +3733,7 @@
       <c r="F156" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G156" s="2">
+      <c r="G156">
         <v>100</v>
       </c>
       <c r="H156" s="1" t="s">
@@ -3760,7 +3759,7 @@
       <c r="F157" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G157" s="2">
+      <c r="G157">
         <v>100</v>
       </c>
       <c r="H157" s="1" t="s">
@@ -3921,7 +3920,7 @@
       <c r="F167" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G167" s="2">
+      <c r="G167">
         <v>100</v>
       </c>
       <c r="H167" s="1" t="s">
@@ -3953,16 +3952,16 @@
       <c r="C169" s="1">
         <v>440</v>
       </c>
-      <c r="D169" s="2">
+      <c r="D169">
         <v>55</v>
       </c>
-      <c r="E169" s="2">
+      <c r="E169">
         <v>5</v>
       </c>
       <c r="F169" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G169" s="2">
+      <c r="G169">
         <v>100</v>
       </c>
       <c r="H169" s="1" t="s">
@@ -4051,7 +4050,7 @@
       <c r="B175" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C175" s="2">
+      <c r="C175">
         <v>390</v>
       </c>
       <c r="D175" s="1">
@@ -4063,7 +4062,7 @@
       <c r="F175" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G175" s="2">
+      <c r="G175">
         <v>100</v>
       </c>
       <c r="H175" s="1" t="s">
@@ -4164,22 +4163,22 @@
       <c r="A182" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B182" s="2" t="s">
+      <c r="B182" t="s">
         <v>193</v>
       </c>
-      <c r="C182" s="2">
+      <c r="C182">
         <v>500</v>
       </c>
-      <c r="D182" s="2">
+      <c r="D182">
         <v>120</v>
       </c>
-      <c r="E182" s="2">
+      <c r="E182">
         <v>4</v>
       </c>
       <c r="F182" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G182" s="2">
+      <c r="G182">
         <v>100</v>
       </c>
     </row>
@@ -4187,22 +4186,22 @@
       <c r="A183" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B183" s="2" t="s">
+      <c r="B183" t="s">
         <v>193</v>
       </c>
-      <c r="C183" s="2">
+      <c r="C183">
         <v>500</v>
       </c>
-      <c r="D183" s="2">
+      <c r="D183">
         <v>35</v>
       </c>
-      <c r="E183" s="2">
+      <c r="E183">
         <v>2</v>
       </c>
       <c r="F183" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G183" s="2">
+      <c r="G183">
         <v>100</v>
       </c>
       <c r="H183" s="1" t="s">
@@ -4213,7 +4212,7 @@
       <c r="A184" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B184" s="2" t="s">
+      <c r="B184" t="s">
         <v>193</v>
       </c>
       <c r="C184" s="1">
@@ -4228,7 +4227,7 @@
       <c r="F184" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G184" s="2">
+      <c r="G184">
         <v>100</v>
       </c>
       <c r="H184" s="1" t="s">
@@ -4239,7 +4238,7 @@
       <c r="A185" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B185" s="2" t="s">
+      <c r="B185" t="s">
         <v>193</v>
       </c>
       <c r="C185" s="1">
@@ -4254,7 +4253,7 @@
       <c r="F185" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G185" s="2">
+      <c r="G185">
         <v>100</v>
       </c>
       <c r="H185" s="1" t="s">
@@ -4265,22 +4264,22 @@
       <c r="A186" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B186" s="2" t="s">
+      <c r="B186" t="s">
         <v>193</v>
       </c>
-      <c r="C186" s="2">
+      <c r="C186">
         <v>350</v>
       </c>
-      <c r="D186" s="2">
+      <c r="D186">
         <v>100</v>
       </c>
-      <c r="E186" s="2">
+      <c r="E186">
         <v>3</v>
       </c>
       <c r="F186" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G186" s="2">
+      <c r="G186">
         <v>50</v>
       </c>
       <c r="H186" s="1" t="s">
@@ -4291,7 +4290,7 @@
       <c r="A187" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B187" s="2" t="s">
+      <c r="B187" t="s">
         <v>193</v>
       </c>
       <c r="C187" s="1">
@@ -4306,171 +4305,171 @@
       <c r="F187" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G187" s="2">
+      <c r="G187">
         <v>100</v>
       </c>
       <c r="H187" s="1" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="188" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A188" s="3" t="s">
+    <row r="188" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A188" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="B188" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C188" s="3">
-        <v>0</v>
-      </c>
-      <c r="D188" s="3">
+      <c r="B188" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C188" s="2">
+        <v>390</v>
+      </c>
+      <c r="D188" s="2">
         <v>50</v>
       </c>
-      <c r="E188" s="3">
-        <v>0</v>
-      </c>
-      <c r="F188" s="3" t="s">
+      <c r="E188" s="2">
+        <v>0</v>
+      </c>
+      <c r="F188" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G188" s="2">
+      <c r="G188">
         <v>100</v>
       </c>
     </row>
-    <row r="189" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A189" s="3" t="s">
+    <row r="189" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A189" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="B189" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C189" s="3">
+      <c r="B189" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C189" s="2">
         <v>370</v>
       </c>
-      <c r="D189" s="3">
+      <c r="D189" s="2">
         <v>150</v>
       </c>
-      <c r="E189" s="3">
-        <v>0</v>
-      </c>
-      <c r="F189" s="3" t="s">
+      <c r="E189" s="2">
+        <v>0</v>
+      </c>
+      <c r="F189" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G189" s="2">
+      <c r="G189">
         <v>100</v>
       </c>
     </row>
-    <row r="190" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A190" s="3" t="s">
+    <row r="190" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A190" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="B190" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C190" s="3">
+      <c r="B190" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C190" s="2">
         <v>490</v>
       </c>
-      <c r="D190" s="3">
+      <c r="D190" s="2">
         <v>50</v>
       </c>
-      <c r="E190" s="3">
+      <c r="E190" s="2">
         <v>5</v>
       </c>
-      <c r="F190" s="3" t="s">
+      <c r="F190" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G190" s="2">
+      <c r="G190">
         <v>100</v>
       </c>
     </row>
-    <row r="191" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A191" s="3" t="s">
+    <row r="191" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A191" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="B191" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C191" s="3">
+      <c r="B191" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C191" s="2">
         <v>330</v>
       </c>
-      <c r="D191" s="3">
+      <c r="D191" s="2">
         <v>50</v>
       </c>
-      <c r="E191" s="3">
-        <v>0</v>
-      </c>
-      <c r="F191" s="3" t="s">
+      <c r="E191" s="2">
+        <v>0</v>
+      </c>
+      <c r="F191" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G191" s="2">
+      <c r="G191">
         <v>100</v>
       </c>
     </row>
-    <row r="192" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A192" s="3" t="s">
+    <row r="192" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A192" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="B192" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C192" s="3">
-        <v>0</v>
-      </c>
-      <c r="D192" s="3">
+      <c r="B192" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C192" s="2">
+        <v>400</v>
+      </c>
+      <c r="D192" s="2">
         <v>55</v>
       </c>
-      <c r="E192" s="3">
-        <v>0</v>
-      </c>
-      <c r="F192" s="3" t="s">
+      <c r="E192" s="2">
+        <v>0</v>
+      </c>
+      <c r="F192" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G192" s="2">
+      <c r="G192">
         <v>100</v>
       </c>
     </row>
-    <row r="193" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A193" s="3" t="s">
+    <row r="193" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A193" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="B193" s="3" t="s">
+      <c r="B193" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C193" s="3">
+      <c r="C193" s="2">
         <v>350</v>
       </c>
-      <c r="D193" s="3">
+      <c r="D193" s="2">
         <v>100</v>
       </c>
-      <c r="E193" s="3">
+      <c r="E193" s="2">
         <v>5</v>
       </c>
-      <c r="F193" s="3" t="s">
+      <c r="F193" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G193" s="2">
+      <c r="G193">
         <v>100</v>
       </c>
     </row>
-    <row r="194" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A194" s="3" t="s">
+    <row r="194" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A194" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="B194" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C194" s="3">
-        <v>0</v>
-      </c>
-      <c r="D194" s="3">
-        <v>1</v>
-      </c>
-      <c r="E194" s="3">
-        <v>0</v>
-      </c>
-      <c r="F194" s="3" t="s">
+      <c r="B194" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C194" s="2">
+        <v>0</v>
+      </c>
+      <c r="D194" s="2">
+        <v>1</v>
+      </c>
+      <c r="E194" s="2">
+        <v>1</v>
+      </c>
+      <c r="F194" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G194" s="2">
+      <c r="G194">
         <v>100</v>
       </c>
     </row>

</xml_diff>